<commit_message>
commited on with latest changes on tickets
</commit_message>
<xml_diff>
--- a/QALegend/src/test/resources/Testdata.xlsx
+++ b/QALegend/src/test/resources/Testdata.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Vincy-Java\eclipse-workspace\QALegend\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\QALegend\QALegend\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F697AE76-A0F6-4254-A2C4-8BCF2787FB48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFDB2A9-8BB7-41A2-90A5-567EAF23382D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event" sheetId="1" r:id="rId1"/>
     <sheet name="Project" sheetId="6" r:id="rId2"/>
-    <sheet name="Message" sheetId="4" r:id="rId3"/>
-    <sheet name="Client" sheetId="5" r:id="rId4"/>
-    <sheet name="Login" sheetId="2" r:id="rId5"/>
-    <sheet name="Note" sheetId="3" r:id="rId6"/>
+    <sheet name="Ticket" sheetId="7" r:id="rId3"/>
+    <sheet name="Message" sheetId="4" r:id="rId4"/>
+    <sheet name="Client" sheetId="5" r:id="rId5"/>
+    <sheet name="Login" sheetId="2" r:id="rId6"/>
+    <sheet name="Note" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -134,13 +135,22 @@
     <t>Chemk Limited</t>
   </si>
   <si>
-    <t>TestSample15</t>
-  </si>
-  <si>
     <t>To add project</t>
   </si>
   <si>
     <t>ProjectHP</t>
+  </si>
+  <si>
+    <t>TicketVM</t>
+  </si>
+  <si>
+    <t>To add ticket</t>
+  </si>
+  <si>
+    <t>TestSample</t>
+  </si>
+  <si>
+    <t>Client</t>
   </si>
 </sst>
 </file>
@@ -567,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B89F88-DDE6-4771-9A33-FA76B68C5783}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,10 +597,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -599,11 +609,52 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D7E2F4-2626-4439-8021-185197768286}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A116E9E8-BA59-440F-8F9F-FAEE8681D2AE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,7 +679,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
@@ -639,7 +690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870C8286-36C1-4AB5-84F8-0795186FA043}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -705,7 +756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA909E66-91C1-41D0-9527-F458B758C4E7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -742,7 +793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A901D2-FFA3-46E3-8EBC-44775E8F2739}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>